<commit_message>
Opciones de formato para el archivo de salida
</commit_message>
<xml_diff>
--- a/Preguntas Ejemplo.xlsx
+++ b/Preguntas Ejemplo.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27531"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/23114eabca2c9a39/Programita multiple choice/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="38" documentId="8_{D50F4479-B71F-4857-9C5E-FFD52260257A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6E441A7B-A2F5-43D4-82A7-411ACC451CAB}"/>
+  <xr:revisionPtr revIDLastSave="41" documentId="8_{D50F4479-B71F-4857-9C5E-FFD52260257A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D0A13C9C-5E30-4C98-9218-B6CC29855809}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-165" windowWidth="29040" windowHeight="15840" xr2:uid="{16C8A16E-4F76-4CE9-8605-C3F6D4C8C054}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="46">
   <si>
     <t>azul</t>
   </si>
@@ -554,10 +554,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E37D0D0-C5D1-4EBC-A8F8-5C757852A676}">
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -722,6 +722,414 @@
         <v>45</v>
       </c>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>12</v>
+      </c>
+      <c r="D12" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13" t="s">
+        <v>23</v>
+      </c>
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>25</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>28</v>
+      </c>
+      <c r="E14" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
+        <v>33</v>
+      </c>
+      <c r="E15" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>36</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" t="s">
+        <v>41</v>
+      </c>
+      <c r="C17" t="s">
+        <v>42</v>
+      </c>
+      <c r="D17" t="s">
+        <v>43</v>
+      </c>
+      <c r="E17" t="s">
+        <v>44</v>
+      </c>
+      <c r="F17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" t="s">
+        <v>1</v>
+      </c>
+      <c r="D18" t="s">
+        <v>2</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19" t="s">
+        <v>8</v>
+      </c>
+      <c r="E19" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>12</v>
+      </c>
+      <c r="D20" t="s">
+        <v>13</v>
+      </c>
+      <c r="E20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" t="s">
+        <v>23</v>
+      </c>
+      <c r="E21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>25</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" t="s">
+        <v>28</v>
+      </c>
+      <c r="E22" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23" t="s">
+        <v>31</v>
+      </c>
+      <c r="C23" t="s">
+        <v>32</v>
+      </c>
+      <c r="D23" t="s">
+        <v>33</v>
+      </c>
+      <c r="E23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>36</v>
+      </c>
+      <c r="B24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>40</v>
+      </c>
+      <c r="B25" t="s">
+        <v>41</v>
+      </c>
+      <c r="C25" t="s">
+        <v>42</v>
+      </c>
+      <c r="D25" t="s">
+        <v>43</v>
+      </c>
+      <c r="E25" t="s">
+        <v>44</v>
+      </c>
+      <c r="F25" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B26" t="s">
+        <v>0</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4</v>
+      </c>
+      <c r="C27" t="s">
+        <v>7</v>
+      </c>
+      <c r="D27" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" t="s">
+        <v>12</v>
+      </c>
+      <c r="D28" t="s">
+        <v>13</v>
+      </c>
+      <c r="E28" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>20</v>
+      </c>
+      <c r="B29" t="s">
+        <v>21</v>
+      </c>
+      <c r="C29" t="s">
+        <v>22</v>
+      </c>
+      <c r="D29" t="s">
+        <v>23</v>
+      </c>
+      <c r="E29" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>25</v>
+      </c>
+      <c r="B30" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" t="s">
+        <v>28</v>
+      </c>
+      <c r="E30" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>31</v>
+      </c>
+      <c r="C31" t="s">
+        <v>32</v>
+      </c>
+      <c r="D31" t="s">
+        <v>33</v>
+      </c>
+      <c r="E31" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>36</v>
+      </c>
+      <c r="B32" t="s">
+        <v>37</v>
+      </c>
+      <c r="C32" t="s">
+        <v>38</v>
+      </c>
+      <c r="D32" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33" t="s">
+        <v>41</v>
+      </c>
+      <c r="C33" t="s">
+        <v>42</v>
+      </c>
+      <c r="D33" t="s">
+        <v>43</v>
+      </c>
+      <c r="E33" t="s">
+        <v>44</v>
+      </c>
+      <c r="F33" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>